<commit_message>
Minor update - GUI
</commit_message>
<xml_diff>
--- a/Structures.xlsx
+++ b/Structures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/cmharwood_uiowa_edu/Documents/Cyclo_UUV/Hexapod GUI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmhar\OneDrive - University of Iowa\Cyclo_UUV\Hexapod GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="215" documentId="8_{2A4F9883-AB71-4FAF-B974-0443F973458B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7444EC8-17F8-43D7-BDBA-C5E2323A73F0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDDC421-585F-4D0A-B495-5B23353D5042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60120" yWindow="-11970" windowWidth="21840" windowHeight="37920" xr2:uid="{260795C8-23F6-4576-8E22-901A1E0FF5FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{260795C8-23F6-4576-8E22-901A1E0FF5FF}"/>
   </bookViews>
   <sheets>
     <sheet name="hex_obj" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="114">
   <si>
     <t>base</t>
   </si>
@@ -373,6 +373,15 @@
   </si>
   <si>
     <t>coordinates of link attachments in base frame - includes yoke offset</t>
+  </si>
+  <si>
+    <t>pose_t_relative</t>
+  </si>
+  <si>
+    <t>end effector pose in world/base frame, relative to current pose.</t>
+  </si>
+  <si>
+    <t>NOTE: relative path is the default. E.g. All motion inputs will be interpreted as being relative to the current pose, unless the motion-planning dialog specifies 'absolute motion', in which case the pose_t array will be modified so that the motions are relative to the hexpod's home position.</t>
   </si>
 </sst>
 </file>
@@ -417,9 +426,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2B9747-9F2A-4439-9C71-7565F0F0F92A}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,23 +1249,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71FEFC3-1FFC-47DB-A624-DB58BB08C9C9}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="56.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -1264,7 +1278,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -1275,7 +1289,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1286,7 +1300,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -1297,91 +1311,105 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
         <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
         <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
         <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
         <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" t="s">
         <v>82</v>
       </c>
       <c r="C11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>92</v>
-      </c>
-      <c r="B12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>71</v>
       </c>
       <c r="B13" t="s">
         <v>94</v>
       </c>
       <c r="C13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>102</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>104</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>